<commit_message>
Add Date Tested and Retest Date columns to UAT Excel
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/app/UAT-TEST-SET.xlsx
+++ b/app/UAT-TEST-SET.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -68,8 +68,12 @@
       <color rgb="00FFFFFF"/>
       <sz val="12"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -92,6 +96,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="002B5F8A"/>
         <bgColor rgb="002B5F8A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="001F4E79"/>
+        <bgColor rgb="001F4E79"/>
       </patternFill>
     </fill>
   </fills>
@@ -172,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -211,6 +221,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,7 +627,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I203"/>
+  <dimension ref="A1:K203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
@@ -625,9 +641,10 @@
     <col width="40" customWidth="1" min="3" max="3"/>
     <col width="45" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
     <col width="10" customWidth="1" min="7" max="7"/>
     <col width="32.33203125" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -697,7 +714,7 @@
       <c r="C7" s="15" t="n"/>
       <c r="D7" s="15" t="n"/>
       <c r="E7" s="15" t="n"/>
-      <c r="F7" s="16" t="n"/>
+      <c r="G7" s="16" t="n"/>
     </row>
     <row r="8" ht="17" customHeight="1">
       <c r="A8" s="3" t="inlineStr">
@@ -725,14 +742,24 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F8" s="3" t="inlineStr">
+      <c r="F8" s="19" t="inlineStr">
+        <is>
+          <t>Date Tested</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G8" s="17" t="inlineStr">
+      <c r="H8" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
+        </is>
+      </c>
+      <c r="I8" s="19" t="inlineStr">
+        <is>
+          <t>Retest Date</t>
         </is>
       </c>
     </row>
@@ -762,7 +789,8 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F9" s="4" t="inlineStr">
+      <c r="F9" s="20" t="n"/>
+      <c r="G9" s="4" t="inlineStr">
         <is>
           <t>Initial Access Issue: First attempt loaded an old deployment. Cleared cache and reloaded — displayed correctly after that.
 UI Fixes Needed:
@@ -772,7 +800,8 @@
 4.  Tagline update — Change "Streamline setup for genetic testing programs" to "Streamline setup for EICI program."</t>
         </is>
       </c>
-      <c r="G9" s="18" t="n"/>
+      <c r="H9" s="18" t="n"/>
+      <c r="I9" s="20" t="n"/>
     </row>
     <row r="10" ht="105" customHeight="1">
       <c r="A10" s="4" t="inlineStr">
@@ -800,13 +829,15 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F10" s="4" t="inlineStr">
+      <c r="F10" s="20" t="n"/>
+      <c r="G10" s="4" t="inlineStr">
         <is>
           <t>Test Actions Performed: Entered Providence email (glen.a.lewis@providence.org) and clicked "Send."
 Results:"Check your email for the Magic Link" confirmation displayed with green success message. PASS.</t>
         </is>
       </c>
-      <c r="G10" s="18" t="n"/>
+      <c r="H10" s="18" t="n"/>
+      <c r="I10" s="20" t="n"/>
     </row>
     <row r="11" ht="90" customHeight="1">
       <c r="A11" s="4" t="inlineStr">
@@ -834,12 +865,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F11" s="4" t="inlineStr">
+      <c r="F11" s="20" t="n"/>
+      <c r="G11" s="4" t="inlineStr">
         <is>
           <t>Browser recognized incomplete email input and displayed prompts indicating what was required. Validation checked in real-time as each character was entered, continuing to flag the email as incomplete until fully formed. PASS.</t>
         </is>
       </c>
-      <c r="G11" s="18" t="n"/>
+      <c r="H11" s="18" t="n"/>
+      <c r="I11" s="20" t="n"/>
     </row>
     <row r="12" ht="409.6" customHeight="1">
       <c r="A12" s="4" t="inlineStr">
@@ -867,7 +900,8 @@
           <t>FAIL</t>
         </is>
       </c>
-      <c r="F12" s="4" t="inlineStr">
+      <c r="F12" s="20" t="n"/>
+      <c r="G12" s="4" t="inlineStr">
         <is>
           <t>Test Actions Performed: Completed full Magic Link sign-in flow after submitting email.
 Results:
@@ -886,8 +920,9 @@
 Actual: User is returned to the login page with no authentication.</t>
         </is>
       </c>
-      <c r="G12" s="18" t="n"/>
-      <c r="H12" s="13" t="inlineStr">
+      <c r="H12" s="18" t="n"/>
+      <c r="I12" s="20" t="n"/>
+      <c r="J12" s="13" t="inlineStr">
         <is>
           <t>UX Improvement: First-Time Double Sign-In Experience
 Priority: Medium
@@ -897,7 +932,7 @@
 2. If the double sign-in must stay — Add clear on-screen messaging after the user clicks "Confirm Email" explaining that they'll need to sign in one more time, and that a second email is on its way.</t>
         </is>
       </c>
-      <c r="I12" s="13" t="inlineStr">
+      <c r="K12" s="13" t="inlineStr">
         <is>
           <t>Test Case 1.3 (Continued): Magic Link Authentication — Existing User
 Test Actions Performed:
@@ -934,10 +969,15 @@
         </is>
       </c>
       <c r="E13" s="4" t="n"/>
-      <c r="F13" s="4" t="n"/>
-      <c r="G13" s="18" t="n"/>
-    </row>
-    <row r="14"/>
+      <c r="F13" s="20" t="n"/>
+      <c r="G13" s="4" t="n"/>
+      <c r="H13" s="18" t="n"/>
+      <c r="I13" s="20" t="n"/>
+    </row>
+    <row r="14">
+      <c r="F14" s="20" t="n"/>
+      <c r="I14" s="20" t="n"/>
+    </row>
     <row r="15" ht="17" customHeight="1">
       <c r="A15" s="11" t="inlineStr">
         <is>
@@ -948,7 +988,9 @@
       <c r="C15" s="15" t="n"/>
       <c r="D15" s="15" t="n"/>
       <c r="E15" s="15" t="n"/>
-      <c r="F15" s="16" t="n"/>
+      <c r="F15" s="20" t="n"/>
+      <c r="G15" s="16" t="n"/>
+      <c r="I15" s="20" t="n"/>
     </row>
     <row r="16" ht="17" customHeight="1">
       <c r="A16" s="3" t="inlineStr">
@@ -976,16 +1018,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F16" s="3" t="inlineStr">
+      <c r="F16" s="20" t="n"/>
+      <c r="G16" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G16" s="17" t="inlineStr">
+      <c r="H16" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I16" s="20" t="n"/>
     </row>
     <row r="17" ht="356" customHeight="1">
       <c r="A17" s="4" t="inlineStr">
@@ -1013,7 +1057,8 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F17" s="4" t="inlineStr">
+      <c r="F17" s="20" t="n"/>
+      <c r="G17" s="4" t="inlineStr">
         <is>
           <t>UX Fixes — Providence Health Clinic Onboarding
 Remove "Providence" text from far left of header.
@@ -1025,7 +1070,8 @@
 Result: All programs appeared as expected. PASS.</t>
         </is>
       </c>
-      <c r="G17" s="18" t="n"/>
+      <c r="H17" s="18" t="n"/>
+      <c r="I17" s="20" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
@@ -1053,8 +1099,10 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F18" s="4" t="n"/>
-      <c r="G18" s="18" t="n"/>
+      <c r="F18" s="20" t="n"/>
+      <c r="G18" s="4" t="n"/>
+      <c r="H18" s="18" t="n"/>
+      <c r="I18" s="20" t="n"/>
     </row>
     <row r="19" ht="75" customHeight="1">
       <c r="A19" s="4" t="inlineStr">
@@ -1082,13 +1130,15 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F19" s="4" t="inlineStr">
+      <c r="F19" s="20" t="n"/>
+      <c r="G19" s="4" t="inlineStr">
         <is>
           <t>Attempted to proceed without selecting a program. Clicked "Next."
 Form blocked progression. Selection box highlighted in red. Error message displayed: "Select Program is required."</t>
         </is>
       </c>
-      <c r="G19" s="18" t="n"/>
+      <c r="H19" s="18" t="n"/>
+      <c r="I19" s="20" t="n"/>
     </row>
     <row r="20" ht="75" customHeight="1">
       <c r="A20" s="4" t="inlineStr">
@@ -1116,15 +1166,20 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F20" s="4" t="inlineStr">
+      <c r="F20" s="20" t="n"/>
+      <c r="G20" s="4" t="inlineStr">
         <is>
           <t>Selected Prevention4ME. Red highlight disappeared. Selection box returned to normal view with green outline. Clicked "Next."
 Successfully navigated to the next page.</t>
         </is>
       </c>
-      <c r="G20" s="18" t="n"/>
-    </row>
-    <row r="21"/>
+      <c r="H20" s="18" t="n"/>
+      <c r="I20" s="20" t="n"/>
+    </row>
+    <row r="21">
+      <c r="F21" s="20" t="n"/>
+      <c r="I21" s="20" t="n"/>
+    </row>
     <row r="22" ht="17" customHeight="1">
       <c r="A22" s="11" t="inlineStr">
         <is>
@@ -1135,7 +1190,9 @@
       <c r="C22" s="15" t="n"/>
       <c r="D22" s="15" t="n"/>
       <c r="E22" s="15" t="n"/>
-      <c r="F22" s="16" t="n"/>
+      <c r="F22" s="20" t="n"/>
+      <c r="G22" s="16" t="n"/>
+      <c r="I22" s="20" t="n"/>
     </row>
     <row r="23" ht="17" customHeight="1">
       <c r="A23" s="3" t="inlineStr">
@@ -1163,16 +1220,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F23" s="3" t="inlineStr">
+      <c r="F23" s="20" t="n"/>
+      <c r="G23" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G23" s="17" t="inlineStr">
+      <c r="H23" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I23" s="20" t="n"/>
     </row>
     <row r="24" ht="135" customHeight="1">
       <c r="A24" s="4" t="inlineStr">
@@ -1200,13 +1259,15 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F24" s="4" t="inlineStr">
+      <c r="F24" s="20" t="n"/>
+      <c r="G24" s="4" t="inlineStr">
         <is>
           <t>Attempted to proceed without completing any required fields. Clicked "Next."
 Form blocked progression. All required fields highlighted in red with corresponding error messages: "Clinic Name is required," "Clinic EPIC ID is required," "Please complete all required address fields," "Timezone is required," "Clinic Office Phone Number is required."</t>
         </is>
       </c>
-      <c r="G24" s="18" t="n"/>
+      <c r="H24" s="18" t="n"/>
+      <c r="I24" s="20" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="4" t="inlineStr">
@@ -1234,8 +1295,10 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F25" s="4" t="n"/>
-      <c r="G25" s="18" t="n"/>
+      <c r="F25" s="20" t="n"/>
+      <c r="G25" s="4" t="n"/>
+      <c r="H25" s="18" t="n"/>
+      <c r="I25" s="20" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="4" t="inlineStr">
@@ -1259,8 +1322,10 @@
         </is>
       </c>
       <c r="E26" s="4" t="n"/>
-      <c r="F26" s="4" t="n"/>
-      <c r="G26" s="18" t="n"/>
+      <c r="F26" s="20" t="n"/>
+      <c r="G26" s="4" t="n"/>
+      <c r="H26" s="18" t="n"/>
+      <c r="I26" s="20" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="4" t="inlineStr">
@@ -1288,12 +1353,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F27" s="4" t="inlineStr">
+      <c r="F27" s="20" t="n"/>
+      <c r="G27" s="4" t="inlineStr">
         <is>
           <t>12345 (for DB reconcillation)</t>
         </is>
       </c>
-      <c r="G27" s="18" t="n"/>
+      <c r="H27" s="18" t="n"/>
+      <c r="I27" s="20" t="n"/>
     </row>
     <row r="28" ht="30" customHeight="1">
       <c r="A28" s="4" t="inlineStr">
@@ -1321,12 +1388,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F28" s="4" t="inlineStr">
+      <c r="F28" s="20" t="n"/>
+      <c r="G28" s="4" t="inlineStr">
         <is>
           <t>123 Any Street, Auburn CA (for DB reconcillation)</t>
         </is>
       </c>
-      <c r="G28" s="18" t="n"/>
+      <c r="H28" s="18" t="n"/>
+      <c r="I28" s="20" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="4" t="inlineStr">
@@ -1354,8 +1423,10 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F29" s="4" t="n"/>
-      <c r="G29" s="18" t="n"/>
+      <c r="F29" s="20" t="n"/>
+      <c r="G29" s="4" t="n"/>
+      <c r="H29" s="18" t="n"/>
+      <c r="I29" s="20" t="n"/>
     </row>
     <row r="30" ht="64" customHeight="1">
       <c r="A30" s="4" t="inlineStr">
@@ -1383,12 +1454,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F30" s="13" t="inlineStr">
+      <c r="F30" s="20" t="n"/>
+      <c r="G30" s="13" t="inlineStr">
         <is>
           <t>Entered a 4-digit zip code. Zip code field remained red. Entire address box remained outlined in red. Could not proceed to next page.</t>
         </is>
       </c>
-      <c r="G30" s="18" t="n"/>
+      <c r="H30" s="18" t="n"/>
+      <c r="I30" s="20" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
@@ -1416,12 +1489,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F31" s="4" t="inlineStr">
+      <c r="F31" s="20" t="n"/>
+      <c r="G31" s="4" t="inlineStr">
         <is>
           <t>97201 (for DB reconsillation)</t>
         </is>
       </c>
-      <c r="G31" s="18" t="n"/>
+      <c r="H31" s="18" t="n"/>
+      <c r="I31" s="20" t="n"/>
     </row>
     <row r="32" ht="30" customHeight="1">
       <c r="A32" s="4" t="inlineStr">
@@ -1449,12 +1524,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F32" s="4" t="inlineStr">
+      <c r="F32" s="20" t="n"/>
+      <c r="G32" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Pacific (for DB reconcillation) </t>
         </is>
       </c>
-      <c r="G32" s="18" t="n"/>
+      <c r="H32" s="18" t="n"/>
+      <c r="I32" s="20" t="n"/>
     </row>
     <row r="33" ht="45" customHeight="1">
       <c r="A33" s="4" t="inlineStr">
@@ -1482,12 +1559,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F33" s="4" t="inlineStr">
+      <c r="F33" s="20" t="n"/>
+      <c r="G33" s="4" t="inlineStr">
         <is>
           <t>Entered partial phone number (555-123). Phone number field remained highlighted in red. Could not proceed to next page.</t>
         </is>
       </c>
-      <c r="G33" s="18" t="n"/>
+      <c r="H33" s="18" t="n"/>
+      <c r="I33" s="20" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="4" t="inlineStr">
@@ -1515,12 +1594,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F34" s="4" t="inlineStr">
+      <c r="F34" s="20" t="n"/>
+      <c r="G34" s="4" t="inlineStr">
         <is>
           <t>555-123-4567 (for DB reconcillation)</t>
         </is>
       </c>
-      <c r="G34" s="18" t="n"/>
+      <c r="H34" s="18" t="n"/>
+      <c r="I34" s="20" t="n"/>
     </row>
     <row r="35" ht="30" customHeight="1">
       <c r="A35" s="4" t="inlineStr">
@@ -1548,8 +1629,10 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F35" s="4" t="n"/>
-      <c r="G35" s="18" t="n"/>
+      <c r="F35" s="20" t="n"/>
+      <c r="G35" s="4" t="n"/>
+      <c r="H35" s="18" t="n"/>
+      <c r="I35" s="20" t="n"/>
     </row>
     <row r="36" ht="30" customHeight="1">
       <c r="A36" s="4" t="inlineStr">
@@ -1577,8 +1660,10 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F36" s="4" t="n"/>
-      <c r="G36" s="18" t="n"/>
+      <c r="F36" s="20" t="n"/>
+      <c r="G36" s="4" t="n"/>
+      <c r="H36" s="18" t="n"/>
+      <c r="I36" s="20" t="n"/>
     </row>
     <row r="37" ht="45" customHeight="1">
       <c r="A37" s="4" t="inlineStr">
@@ -1606,12 +1691,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F37" s="4" t="inlineStr">
+      <c r="F37" s="20" t="n"/>
+      <c r="G37" s="4" t="inlineStr">
         <is>
           <t>Entered partial phone number (555-123). Phone number field remained highlighted in red. Could not proceed to next page.</t>
         </is>
       </c>
-      <c r="G37" s="18" t="n"/>
+      <c r="H37" s="18" t="n"/>
+      <c r="I37" s="20" t="n"/>
     </row>
     <row r="38">
       <c r="A38" s="4" t="inlineStr">
@@ -1639,8 +1726,10 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F38" s="4" t="n"/>
-      <c r="G38" s="18" t="n"/>
+      <c r="F38" s="20" t="n"/>
+      <c r="G38" s="4" t="n"/>
+      <c r="H38" s="18" t="n"/>
+      <c r="I38" s="20" t="n"/>
     </row>
     <row r="39" ht="30" customHeight="1">
       <c r="A39" s="4" t="inlineStr">
@@ -1668,8 +1757,10 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F39" s="4" t="n"/>
-      <c r="G39" s="18" t="n"/>
+      <c r="F39" s="20" t="n"/>
+      <c r="G39" s="4" t="n"/>
+      <c r="H39" s="18" t="n"/>
+      <c r="I39" s="20" t="n"/>
     </row>
     <row r="40" ht="30" customHeight="1">
       <c r="A40" s="4" t="inlineStr">
@@ -1697,10 +1788,15 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F40" s="4" t="n"/>
-      <c r="G40" s="18" t="n"/>
-    </row>
-    <row r="41"/>
+      <c r="F40" s="20" t="n"/>
+      <c r="G40" s="4" t="n"/>
+      <c r="H40" s="18" t="n"/>
+      <c r="I40" s="20" t="n"/>
+    </row>
+    <row r="41">
+      <c r="F41" s="20" t="n"/>
+      <c r="I41" s="20" t="n"/>
+    </row>
     <row r="42" ht="17" customHeight="1">
       <c r="A42" s="11" t="inlineStr">
         <is>
@@ -1711,7 +1807,9 @@
       <c r="C42" s="15" t="n"/>
       <c r="D42" s="15" t="n"/>
       <c r="E42" s="15" t="n"/>
-      <c r="F42" s="16" t="n"/>
+      <c r="F42" s="20" t="n"/>
+      <c r="G42" s="16" t="n"/>
+      <c r="I42" s="20" t="n"/>
     </row>
     <row r="43" ht="17" customHeight="1">
       <c r="A43" s="3" t="inlineStr">
@@ -1739,16 +1837,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F43" s="3" t="inlineStr">
+      <c r="F43" s="20" t="n"/>
+      <c r="G43" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G43" s="17" t="inlineStr">
+      <c r="H43" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I43" s="20" t="n"/>
     </row>
     <row r="44" ht="30" customHeight="1">
       <c r="A44" s="4" t="inlineStr">
@@ -1776,8 +1876,10 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F44" s="4" t="n"/>
-      <c r="G44" s="18" t="n"/>
+      <c r="F44" s="20" t="n"/>
+      <c r="G44" s="4" t="n"/>
+      <c r="H44" s="18" t="n"/>
+      <c r="I44" s="20" t="n"/>
     </row>
     <row r="45" ht="80" customHeight="1">
       <c r="A45" s="4" t="inlineStr">
@@ -1805,12 +1907,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F45" s="13" t="inlineStr">
+      <c r="F45" s="20" t="n"/>
+      <c r="G45" s="13" t="inlineStr">
         <is>
           <t>Left all contact fields blank (covers sub-tests 4.2, 4.8, 4.9). Attempted to navigate to next page. All fields highlighted in red as required. Could not proceed.</t>
         </is>
       </c>
-      <c r="G45" s="18" t="n"/>
+      <c r="H45" s="18" t="n"/>
+      <c r="I45" s="20" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="4" t="inlineStr">
@@ -1838,12 +1942,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F46" s="4" t="inlineStr">
+      <c r="F46" s="20" t="n"/>
+      <c r="G46" s="4" t="inlineStr">
         <is>
           <t>Jane Smith (for DB reconcillation)</t>
         </is>
       </c>
-      <c r="G46" s="18" t="n"/>
+      <c r="H46" s="18" t="n"/>
+      <c r="I46" s="20" t="n"/>
     </row>
     <row r="47" ht="64" customHeight="1">
       <c r="A47" s="4" t="inlineStr">
@@ -1871,12 +1977,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F47" s="13" t="inlineStr">
+      <c r="F47" s="20" t="n"/>
+      <c r="G47" s="13" t="inlineStr">
         <is>
           <t>Entered improperly formatted email. Form blocked navigation to next page until a properly formatted email was entered.</t>
         </is>
       </c>
-      <c r="G47" s="18" t="n"/>
+      <c r="H47" s="18" t="n"/>
+      <c r="I47" s="20" t="n"/>
     </row>
     <row r="48" ht="195" customHeight="1">
       <c r="A48" s="4" t="inlineStr">
@@ -1904,14 +2012,16 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F48" s="4" t="inlineStr">
+      <c r="F48" s="20" t="n"/>
+      <c r="G48" s="4" t="inlineStr">
         <is>
           <t>Entered incomplete phone number. Form blocked navigation to next page.
 PASS — but with UX issue noted below.     UX Improvement — Phone Number Error Indicator
 When an incomplete phone number is entered, the form correctly blocks navigation but does not highlight the phone number field as an error. While the field may not be required, if the format is invalid, there should be a visual indication that it needs correction. Currently the user has no feedback on what's blocking them.</t>
         </is>
       </c>
-      <c r="G48" s="18" t="n"/>
+      <c r="H48" s="18" t="n"/>
+      <c r="I48" s="20" t="n"/>
     </row>
     <row r="49" ht="30" customHeight="1">
       <c r="A49" s="4" t="inlineStr">
@@ -1939,8 +2049,10 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F49" s="4" t="n"/>
-      <c r="G49" s="18" t="n"/>
+      <c r="F49" s="20" t="n"/>
+      <c r="G49" s="4" t="n"/>
+      <c r="H49" s="18" t="n"/>
+      <c r="I49" s="20" t="n"/>
     </row>
     <row r="50" ht="30" customHeight="1">
       <c r="A50" s="4" t="inlineStr">
@@ -1968,8 +2080,10 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F50" s="4" t="n"/>
-      <c r="G50" s="18" t="n"/>
+      <c r="F50" s="20" t="n"/>
+      <c r="G50" s="4" t="n"/>
+      <c r="H50" s="18" t="n"/>
+      <c r="I50" s="20" t="n"/>
     </row>
     <row r="51" ht="80" customHeight="1">
       <c r="A51" s="4" t="inlineStr">
@@ -1997,12 +2111,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F51" s="14" t="inlineStr">
+      <c r="F51" s="20" t="n"/>
+      <c r="G51" s="14" t="inlineStr">
         <is>
           <t>Left all contact fields blank (covers sub-tests 4.2, 4.8, 4.9). Attempted to navigate to next page. All fields highlighted in red as required. Could not proceed.</t>
         </is>
       </c>
-      <c r="G51" s="18" t="n"/>
+      <c r="H51" s="18" t="n"/>
+      <c r="I51" s="20" t="n"/>
     </row>
     <row r="52" ht="96" customHeight="1">
       <c r="A52" s="4" t="inlineStr">
@@ -2030,12 +2146,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F52" s="14" t="inlineStr">
+      <c r="F52" s="20" t="n"/>
+      <c r="G52" s="14" t="inlineStr">
         <is>
           <t>Left all contact fields blank (covers sub-tests 4.2, 4.8, 4.9). Attempted to navigate to next page. All fields highlighted in red as required. Could not proceed. Jon Doe (for DB reconcillation)</t>
         </is>
       </c>
-      <c r="G52" s="18" t="n"/>
+      <c r="H52" s="18" t="n"/>
+      <c r="I52" s="20" t="n"/>
     </row>
     <row r="53" ht="30" customHeight="1">
       <c r="A53" s="4" t="inlineStr">
@@ -2063,8 +2181,10 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F53" s="4" t="n"/>
-      <c r="G53" s="18" t="n"/>
+      <c r="F53" s="20" t="n"/>
+      <c r="G53" s="4" t="n"/>
+      <c r="H53" s="18" t="n"/>
+      <c r="I53" s="20" t="n"/>
     </row>
     <row r="54" ht="30" customHeight="1">
       <c r="A54" s="4" t="inlineStr">
@@ -2092,8 +2212,10 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F54" s="4" t="n"/>
-      <c r="G54" s="18" t="n"/>
+      <c r="F54" s="20" t="n"/>
+      <c r="G54" s="4" t="n"/>
+      <c r="H54" s="18" t="n"/>
+      <c r="I54" s="20" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="4" t="inlineStr">
@@ -2121,10 +2243,15 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F55" s="4" t="n"/>
-      <c r="G55" s="18" t="n"/>
-    </row>
-    <row r="56"/>
+      <c r="F55" s="20" t="n"/>
+      <c r="G55" s="4" t="n"/>
+      <c r="H55" s="18" t="n"/>
+      <c r="I55" s="20" t="n"/>
+    </row>
+    <row r="56">
+      <c r="F56" s="20" t="n"/>
+      <c r="I56" s="20" t="n"/>
+    </row>
     <row r="57" ht="17" customHeight="1">
       <c r="A57" s="11" t="inlineStr">
         <is>
@@ -2135,7 +2262,9 @@
       <c r="C57" s="15" t="n"/>
       <c r="D57" s="15" t="n"/>
       <c r="E57" s="15" t="n"/>
-      <c r="F57" s="16" t="n"/>
+      <c r="F57" s="20" t="n"/>
+      <c r="G57" s="16" t="n"/>
+      <c r="I57" s="20" t="n"/>
     </row>
     <row r="58" ht="17" customHeight="1">
       <c r="A58" s="3" t="inlineStr">
@@ -2163,16 +2292,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F58" s="3" t="inlineStr">
+      <c r="F58" s="20" t="n"/>
+      <c r="G58" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G58" s="17" t="inlineStr">
+      <c r="H58" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I58" s="20" t="n"/>
     </row>
     <row r="59" ht="30" customHeight="1">
       <c r="A59" s="4" t="inlineStr">
@@ -2200,12 +2331,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F59" s="4" t="inlineStr">
+      <c r="F59" s="20" t="n"/>
+      <c r="G59" s="4" t="inlineStr">
         <is>
           <t>All fields displayed properly. Able to navigate to next page.</t>
         </is>
       </c>
-      <c r="G59" s="18" t="n"/>
+      <c r="H59" s="18" t="n"/>
+      <c r="I59" s="20" t="n"/>
     </row>
     <row r="60" ht="30" customHeight="1">
       <c r="A60" s="4" t="inlineStr">
@@ -2233,12 +2366,14 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr">
+      <c r="F60" s="20" t="n"/>
+      <c r="G60" t="inlineStr">
         <is>
           <t>All stakeholder groups rendered correctly.</t>
         </is>
       </c>
-      <c r="G60" s="18" t="n"/>
+      <c r="H60" s="18" t="n"/>
+      <c r="I60" s="20" t="n"/>
     </row>
     <row r="61" ht="195" customHeight="1">
       <c r="A61" s="4" t="inlineStr">
@@ -2266,13 +2401,15 @@
           <t>PASS</t>
         </is>
       </c>
-      <c r="F61" s="4" t="inlineStr">
+      <c r="F61" s="20" t="n"/>
+      <c r="G61" s="4" t="inlineStr">
         <is>
           <t>Email and phone number fields validated properly. Could not navigate to next page without properly formatted email or phone number.
 PASS — but with UX issue noted below.  Same behavior as previous contact section. When clicking "Next" with an improperly formatted email or phone number, the form blocks navigation but provides no visual indication of which field is causing the issue. No error highlighting, helper icon, or tooltip appears. User must scroll to top to manually identify the problem.</t>
         </is>
       </c>
-      <c r="G61" s="18" t="n"/>
+      <c r="H61" s="18" t="n"/>
+      <c r="I61" s="20" t="n"/>
     </row>
     <row r="62" ht="30" customHeight="1">
       <c r="A62" s="4" t="inlineStr">
@@ -2296,14 +2433,19 @@
         </is>
       </c>
       <c r="E62" s="4" t="n"/>
-      <c r="F62" s="4" t="inlineStr">
+      <c r="F62" s="20" t="n"/>
+      <c r="G62" s="4" t="inlineStr">
         <is>
           <t xml:space="preserve">Robert Mill (for db reconcillaiton) check as ordering provider. </t>
         </is>
       </c>
-      <c r="G62" s="18" t="n"/>
-    </row>
-    <row r="63"/>
+      <c r="H62" s="18" t="n"/>
+      <c r="I62" s="20" t="n"/>
+    </row>
+    <row r="63">
+      <c r="F63" s="20" t="n"/>
+      <c r="I63" s="20" t="n"/>
+    </row>
     <row r="64" ht="17" customHeight="1">
       <c r="A64" s="11" t="inlineStr">
         <is>
@@ -2314,7 +2456,9 @@
       <c r="C64" s="15" t="n"/>
       <c r="D64" s="15" t="n"/>
       <c r="E64" s="15" t="n"/>
-      <c r="F64" s="16" t="n"/>
+      <c r="F64" s="20" t="n"/>
+      <c r="G64" s="16" t="n"/>
+      <c r="I64" s="20" t="n"/>
     </row>
     <row r="65" ht="17" customHeight="1">
       <c r="A65" s="3" t="inlineStr">
@@ -2342,16 +2486,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F65" s="3" t="inlineStr">
+      <c r="F65" s="20" t="n"/>
+      <c r="G65" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G65" s="17" t="inlineStr">
+      <c r="H65" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I65" s="20" t="n"/>
     </row>
     <row r="66">
       <c r="A66" s="4" t="inlineStr">
@@ -2375,8 +2521,10 @@
         </is>
       </c>
       <c r="E66" s="4" t="n"/>
-      <c r="F66" s="4" t="n"/>
-      <c r="G66" s="18" t="n"/>
+      <c r="F66" s="20" t="n"/>
+      <c r="G66" s="4" t="n"/>
+      <c r="H66" s="18" t="n"/>
+      <c r="I66" s="20" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="4" t="inlineStr">
@@ -2400,8 +2548,10 @@
         </is>
       </c>
       <c r="E67" s="4" t="n"/>
-      <c r="F67" s="4" t="n"/>
-      <c r="G67" s="18" t="n"/>
+      <c r="F67" s="20" t="n"/>
+      <c r="G67" s="4" t="n"/>
+      <c r="H67" s="18" t="n"/>
+      <c r="I67" s="20" t="n"/>
     </row>
     <row r="68" ht="30" customHeight="1">
       <c r="A68" s="4" t="inlineStr">
@@ -2425,8 +2575,10 @@
         </is>
       </c>
       <c r="E68" s="4" t="n"/>
-      <c r="F68" s="4" t="n"/>
-      <c r="G68" s="18" t="n"/>
+      <c r="F68" s="20" t="n"/>
+      <c r="G68" s="4" t="n"/>
+      <c r="H68" s="18" t="n"/>
+      <c r="I68" s="20" t="n"/>
     </row>
     <row r="69" ht="30" customHeight="1">
       <c r="A69" s="4" t="inlineStr">
@@ -2450,8 +2602,10 @@
         </is>
       </c>
       <c r="E69" s="4" t="n"/>
-      <c r="F69" s="4" t="n"/>
-      <c r="G69" s="18" t="n"/>
+      <c r="F69" s="20" t="n"/>
+      <c r="G69" s="4" t="n"/>
+      <c r="H69" s="18" t="n"/>
+      <c r="I69" s="20" t="n"/>
     </row>
     <row r="70">
       <c r="A70" s="4" t="inlineStr">
@@ -2475,8 +2629,10 @@
         </is>
       </c>
       <c r="E70" s="4" t="n"/>
-      <c r="F70" s="4" t="n"/>
-      <c r="G70" s="18" t="n"/>
+      <c r="F70" s="20" t="n"/>
+      <c r="G70" s="4" t="n"/>
+      <c r="H70" s="18" t="n"/>
+      <c r="I70" s="20" t="n"/>
     </row>
     <row r="71" ht="30" customHeight="1">
       <c r="A71" s="4" t="inlineStr">
@@ -2500,8 +2656,10 @@
         </is>
       </c>
       <c r="E71" s="4" t="n"/>
-      <c r="F71" s="4" t="n"/>
-      <c r="G71" s="18" t="n"/>
+      <c r="F71" s="20" t="n"/>
+      <c r="G71" s="4" t="n"/>
+      <c r="H71" s="18" t="n"/>
+      <c r="I71" s="20" t="n"/>
     </row>
     <row r="72">
       <c r="A72" s="4" t="inlineStr">
@@ -2525,8 +2683,10 @@
         </is>
       </c>
       <c r="E72" s="4" t="n"/>
-      <c r="F72" s="4" t="n"/>
-      <c r="G72" s="18" t="n"/>
+      <c r="F72" s="20" t="n"/>
+      <c r="G72" s="4" t="n"/>
+      <c r="H72" s="18" t="n"/>
+      <c r="I72" s="20" t="n"/>
     </row>
     <row r="73">
       <c r="A73" s="4" t="inlineStr">
@@ -2550,8 +2710,10 @@
         </is>
       </c>
       <c r="E73" s="4" t="n"/>
-      <c r="F73" s="4" t="n"/>
-      <c r="G73" s="18" t="n"/>
+      <c r="F73" s="20" t="n"/>
+      <c r="G73" s="4" t="n"/>
+      <c r="H73" s="18" t="n"/>
+      <c r="I73" s="20" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="4" t="inlineStr">
@@ -2575,8 +2737,10 @@
         </is>
       </c>
       <c r="E74" s="4" t="n"/>
-      <c r="F74" s="4" t="n"/>
-      <c r="G74" s="18" t="n"/>
+      <c r="F74" s="20" t="n"/>
+      <c r="G74" s="4" t="n"/>
+      <c r="H74" s="18" t="n"/>
+      <c r="I74" s="20" t="n"/>
     </row>
     <row r="75">
       <c r="A75" s="4" t="inlineStr">
@@ -2600,8 +2764,10 @@
         </is>
       </c>
       <c r="E75" s="4" t="n"/>
-      <c r="F75" s="4" t="n"/>
-      <c r="G75" s="18" t="n"/>
+      <c r="F75" s="20" t="n"/>
+      <c r="G75" s="4" t="n"/>
+      <c r="H75" s="18" t="n"/>
+      <c r="I75" s="20" t="n"/>
     </row>
     <row r="76" ht="30" customHeight="1">
       <c r="A76" s="4" t="inlineStr">
@@ -2625,8 +2791,10 @@
         </is>
       </c>
       <c r="E76" s="4" t="n"/>
-      <c r="F76" s="4" t="n"/>
-      <c r="G76" s="18" t="n"/>
+      <c r="F76" s="20" t="n"/>
+      <c r="G76" s="4" t="n"/>
+      <c r="H76" s="18" t="n"/>
+      <c r="I76" s="20" t="n"/>
     </row>
     <row r="77">
       <c r="A77" s="4" t="inlineStr">
@@ -2650,8 +2818,10 @@
         </is>
       </c>
       <c r="E77" s="4" t="n"/>
-      <c r="F77" s="4" t="n"/>
-      <c r="G77" s="18" t="n"/>
+      <c r="F77" s="20" t="n"/>
+      <c r="G77" s="4" t="n"/>
+      <c r="H77" s="18" t="n"/>
+      <c r="I77" s="20" t="n"/>
     </row>
     <row r="78">
       <c r="A78" s="4" t="inlineStr">
@@ -2675,8 +2845,10 @@
         </is>
       </c>
       <c r="E78" s="4" t="n"/>
-      <c r="F78" s="4" t="n"/>
-      <c r="G78" s="18" t="n"/>
+      <c r="F78" s="20" t="n"/>
+      <c r="G78" s="4" t="n"/>
+      <c r="H78" s="18" t="n"/>
+      <c r="I78" s="20" t="n"/>
     </row>
     <row r="79">
       <c r="A79" s="4" t="inlineStr">
@@ -2700,8 +2872,10 @@
         </is>
       </c>
       <c r="E79" s="4" t="n"/>
-      <c r="F79" s="4" t="n"/>
-      <c r="G79" s="18" t="n"/>
+      <c r="F79" s="20" t="n"/>
+      <c r="G79" s="4" t="n"/>
+      <c r="H79" s="18" t="n"/>
+      <c r="I79" s="20" t="n"/>
     </row>
     <row r="80">
       <c r="A80" s="4" t="inlineStr">
@@ -2725,8 +2899,10 @@
         </is>
       </c>
       <c r="E80" s="4" t="n"/>
-      <c r="F80" s="4" t="n"/>
-      <c r="G80" s="18" t="n"/>
+      <c r="F80" s="20" t="n"/>
+      <c r="G80" s="4" t="n"/>
+      <c r="H80" s="18" t="n"/>
+      <c r="I80" s="20" t="n"/>
     </row>
     <row r="81">
       <c r="A81" s="4" t="inlineStr">
@@ -2750,8 +2926,10 @@
         </is>
       </c>
       <c r="E81" s="4" t="n"/>
-      <c r="F81" s="4" t="n"/>
-      <c r="G81" s="18" t="n"/>
+      <c r="F81" s="20" t="n"/>
+      <c r="G81" s="4" t="n"/>
+      <c r="H81" s="18" t="n"/>
+      <c r="I81" s="20" t="n"/>
     </row>
     <row r="82">
       <c r="A82" s="4" t="inlineStr">
@@ -2775,8 +2953,10 @@
         </is>
       </c>
       <c r="E82" s="4" t="n"/>
-      <c r="F82" s="4" t="n"/>
-      <c r="G82" s="18" t="n"/>
+      <c r="F82" s="20" t="n"/>
+      <c r="G82" s="4" t="n"/>
+      <c r="H82" s="18" t="n"/>
+      <c r="I82" s="20" t="n"/>
     </row>
     <row r="83" ht="30" customHeight="1">
       <c r="A83" s="4" t="inlineStr">
@@ -2800,10 +2980,15 @@
         </is>
       </c>
       <c r="E83" s="4" t="n"/>
-      <c r="F83" s="4" t="n"/>
-      <c r="G83" s="18" t="n"/>
-    </row>
-    <row r="84"/>
+      <c r="F83" s="20" t="n"/>
+      <c r="G83" s="4" t="n"/>
+      <c r="H83" s="18" t="n"/>
+      <c r="I83" s="20" t="n"/>
+    </row>
+    <row r="84">
+      <c r="F84" s="20" t="n"/>
+      <c r="I84" s="20" t="n"/>
+    </row>
     <row r="85" ht="17" customHeight="1">
       <c r="A85" s="11" t="inlineStr">
         <is>
@@ -2814,7 +2999,9 @@
       <c r="C85" s="15" t="n"/>
       <c r="D85" s="15" t="n"/>
       <c r="E85" s="15" t="n"/>
-      <c r="F85" s="16" t="n"/>
+      <c r="F85" s="20" t="n"/>
+      <c r="G85" s="16" t="n"/>
+      <c r="I85" s="20" t="n"/>
     </row>
     <row r="86" ht="17" customHeight="1">
       <c r="A86" s="3" t="inlineStr">
@@ -2842,16 +3029,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F86" s="3" t="inlineStr">
+      <c r="F86" s="20" t="n"/>
+      <c r="G86" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G86" s="17" t="inlineStr">
+      <c r="H86" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I86" s="20" t="n"/>
     </row>
     <row r="87">
       <c r="A87" s="4" t="inlineStr">
@@ -2875,8 +3064,10 @@
         </is>
       </c>
       <c r="E87" s="4" t="n"/>
-      <c r="F87" s="4" t="n"/>
-      <c r="G87" s="18" t="n"/>
+      <c r="F87" s="20" t="n"/>
+      <c r="G87" s="4" t="n"/>
+      <c r="H87" s="18" t="n"/>
+      <c r="I87" s="20" t="n"/>
     </row>
     <row r="88" ht="30" customHeight="1">
       <c r="A88" s="4" t="inlineStr">
@@ -2900,8 +3091,10 @@
         </is>
       </c>
       <c r="E88" s="4" t="n"/>
-      <c r="F88" s="4" t="n"/>
-      <c r="G88" s="18" t="n"/>
+      <c r="F88" s="20" t="n"/>
+      <c r="G88" s="4" t="n"/>
+      <c r="H88" s="18" t="n"/>
+      <c r="I88" s="20" t="n"/>
     </row>
     <row r="89">
       <c r="A89" s="4" t="inlineStr">
@@ -2925,8 +3118,10 @@
         </is>
       </c>
       <c r="E89" s="4" t="n"/>
-      <c r="F89" s="4" t="n"/>
-      <c r="G89" s="18" t="n"/>
+      <c r="F89" s="20" t="n"/>
+      <c r="G89" s="4" t="n"/>
+      <c r="H89" s="18" t="n"/>
+      <c r="I89" s="20" t="n"/>
     </row>
     <row r="90">
       <c r="A90" s="4" t="inlineStr">
@@ -2950,8 +3145,10 @@
         </is>
       </c>
       <c r="E90" s="4" t="n"/>
-      <c r="F90" s="4" t="n"/>
-      <c r="G90" s="18" t="n"/>
+      <c r="F90" s="20" t="n"/>
+      <c r="G90" s="4" t="n"/>
+      <c r="H90" s="18" t="n"/>
+      <c r="I90" s="20" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="4" t="inlineStr">
@@ -2975,8 +3172,10 @@
         </is>
       </c>
       <c r="E91" s="4" t="n"/>
-      <c r="F91" s="4" t="n"/>
-      <c r="G91" s="18" t="n"/>
+      <c r="F91" s="20" t="n"/>
+      <c r="G91" s="4" t="n"/>
+      <c r="H91" s="18" t="n"/>
+      <c r="I91" s="20" t="n"/>
     </row>
     <row r="92">
       <c r="A92" s="4" t="inlineStr">
@@ -3000,8 +3199,10 @@
         </is>
       </c>
       <c r="E92" s="4" t="n"/>
-      <c r="F92" s="4" t="n"/>
-      <c r="G92" s="18" t="n"/>
+      <c r="F92" s="20" t="n"/>
+      <c r="G92" s="4" t="n"/>
+      <c r="H92" s="18" t="n"/>
+      <c r="I92" s="20" t="n"/>
     </row>
     <row r="93" ht="30" customHeight="1">
       <c r="A93" s="4" t="inlineStr">
@@ -3025,10 +3226,15 @@
         </is>
       </c>
       <c r="E93" s="4" t="n"/>
-      <c r="F93" s="4" t="n"/>
-      <c r="G93" s="18" t="n"/>
-    </row>
-    <row r="94"/>
+      <c r="F93" s="20" t="n"/>
+      <c r="G93" s="4" t="n"/>
+      <c r="H93" s="18" t="n"/>
+      <c r="I93" s="20" t="n"/>
+    </row>
+    <row r="94">
+      <c r="F94" s="20" t="n"/>
+      <c r="I94" s="20" t="n"/>
+    </row>
     <row r="95" ht="17" customHeight="1">
       <c r="A95" s="11" t="inlineStr">
         <is>
@@ -3039,7 +3245,9 @@
       <c r="C95" s="15" t="n"/>
       <c r="D95" s="15" t="n"/>
       <c r="E95" s="15" t="n"/>
-      <c r="F95" s="16" t="n"/>
+      <c r="F95" s="20" t="n"/>
+      <c r="G95" s="16" t="n"/>
+      <c r="I95" s="20" t="n"/>
     </row>
     <row r="96" ht="17" customHeight="1">
       <c r="A96" s="3" t="inlineStr">
@@ -3067,16 +3275,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F96" s="3" t="inlineStr">
+      <c r="F96" s="20" t="n"/>
+      <c r="G96" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G96" s="17" t="inlineStr">
+      <c r="H96" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I96" s="20" t="n"/>
     </row>
     <row r="97">
       <c r="A97" s="4" t="inlineStr">
@@ -3100,8 +3310,10 @@
         </is>
       </c>
       <c r="E97" s="4" t="n"/>
-      <c r="F97" s="4" t="n"/>
-      <c r="G97" s="18" t="n"/>
+      <c r="F97" s="20" t="n"/>
+      <c r="G97" s="4" t="n"/>
+      <c r="H97" s="18" t="n"/>
+      <c r="I97" s="20" t="n"/>
     </row>
     <row r="98" ht="30" customHeight="1">
       <c r="A98" s="4" t="inlineStr">
@@ -3125,8 +3337,10 @@
         </is>
       </c>
       <c r="E98" s="4" t="n"/>
-      <c r="F98" s="4" t="n"/>
-      <c r="G98" s="18" t="n"/>
+      <c r="F98" s="20" t="n"/>
+      <c r="G98" s="4" t="n"/>
+      <c r="H98" s="18" t="n"/>
+      <c r="I98" s="20" t="n"/>
     </row>
     <row r="99" ht="30" customHeight="1">
       <c r="A99" s="4" t="inlineStr">
@@ -3150,8 +3364,10 @@
         </is>
       </c>
       <c r="E99" s="4" t="n"/>
-      <c r="F99" s="4" t="n"/>
-      <c r="G99" s="18" t="n"/>
+      <c r="F99" s="20" t="n"/>
+      <c r="G99" s="4" t="n"/>
+      <c r="H99" s="18" t="n"/>
+      <c r="I99" s="20" t="n"/>
     </row>
     <row r="100">
       <c r="A100" s="4" t="inlineStr">
@@ -3175,8 +3391,10 @@
         </is>
       </c>
       <c r="E100" s="4" t="n"/>
-      <c r="F100" s="4" t="n"/>
-      <c r="G100" s="18" t="n"/>
+      <c r="F100" s="20" t="n"/>
+      <c r="G100" s="4" t="n"/>
+      <c r="H100" s="18" t="n"/>
+      <c r="I100" s="20" t="n"/>
     </row>
     <row r="101">
       <c r="A101" s="4" t="inlineStr">
@@ -3200,8 +3418,10 @@
         </is>
       </c>
       <c r="E101" s="4" t="n"/>
-      <c r="F101" s="4" t="n"/>
-      <c r="G101" s="18" t="n"/>
+      <c r="F101" s="20" t="n"/>
+      <c r="G101" s="4" t="n"/>
+      <c r="H101" s="18" t="n"/>
+      <c r="I101" s="20" t="n"/>
     </row>
     <row r="102">
       <c r="A102" s="4" t="inlineStr">
@@ -3225,8 +3445,10 @@
         </is>
       </c>
       <c r="E102" s="4" t="n"/>
-      <c r="F102" s="4" t="n"/>
-      <c r="G102" s="18" t="n"/>
+      <c r="F102" s="20" t="n"/>
+      <c r="G102" s="4" t="n"/>
+      <c r="H102" s="18" t="n"/>
+      <c r="I102" s="20" t="n"/>
     </row>
     <row r="103">
       <c r="A103" s="4" t="inlineStr">
@@ -3250,8 +3472,10 @@
         </is>
       </c>
       <c r="E103" s="4" t="n"/>
-      <c r="F103" s="4" t="n"/>
-      <c r="G103" s="18" t="n"/>
+      <c r="F103" s="20" t="n"/>
+      <c r="G103" s="4" t="n"/>
+      <c r="H103" s="18" t="n"/>
+      <c r="I103" s="20" t="n"/>
     </row>
     <row r="104">
       <c r="A104" s="4" t="inlineStr">
@@ -3275,8 +3499,10 @@
         </is>
       </c>
       <c r="E104" s="4" t="n"/>
-      <c r="F104" s="4" t="n"/>
-      <c r="G104" s="18" t="n"/>
+      <c r="F104" s="20" t="n"/>
+      <c r="G104" s="4" t="n"/>
+      <c r="H104" s="18" t="n"/>
+      <c r="I104" s="20" t="n"/>
     </row>
     <row r="105">
       <c r="A105" s="4" t="inlineStr">
@@ -3300,8 +3526,10 @@
         </is>
       </c>
       <c r="E105" s="4" t="n"/>
-      <c r="F105" s="4" t="n"/>
-      <c r="G105" s="18" t="n"/>
+      <c r="F105" s="20" t="n"/>
+      <c r="G105" s="4" t="n"/>
+      <c r="H105" s="18" t="n"/>
+      <c r="I105" s="20" t="n"/>
     </row>
     <row r="106">
       <c r="A106" s="4" t="inlineStr">
@@ -3325,8 +3553,10 @@
         </is>
       </c>
       <c r="E106" s="4" t="n"/>
-      <c r="F106" s="4" t="n"/>
-      <c r="G106" s="18" t="n"/>
+      <c r="F106" s="20" t="n"/>
+      <c r="G106" s="4" t="n"/>
+      <c r="H106" s="18" t="n"/>
+      <c r="I106" s="20" t="n"/>
     </row>
     <row r="107">
       <c r="A107" s="4" t="inlineStr">
@@ -3350,10 +3580,15 @@
         </is>
       </c>
       <c r="E107" s="4" t="n"/>
-      <c r="F107" s="4" t="n"/>
-      <c r="G107" s="18" t="n"/>
-    </row>
-    <row r="108"/>
+      <c r="F107" s="20" t="n"/>
+      <c r="G107" s="4" t="n"/>
+      <c r="H107" s="18" t="n"/>
+      <c r="I107" s="20" t="n"/>
+    </row>
+    <row r="108">
+      <c r="F108" s="20" t="n"/>
+      <c r="I108" s="20" t="n"/>
+    </row>
     <row r="109" ht="17" customHeight="1">
       <c r="A109" s="11" t="inlineStr">
         <is>
@@ -3364,7 +3599,9 @@
       <c r="C109" s="15" t="n"/>
       <c r="D109" s="15" t="n"/>
       <c r="E109" s="15" t="n"/>
-      <c r="F109" s="16" t="n"/>
+      <c r="F109" s="20" t="n"/>
+      <c r="G109" s="16" t="n"/>
+      <c r="I109" s="20" t="n"/>
     </row>
     <row r="110" ht="17" customHeight="1">
       <c r="A110" s="3" t="inlineStr">
@@ -3392,16 +3629,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F110" s="3" t="inlineStr">
+      <c r="F110" s="20" t="n"/>
+      <c r="G110" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G110" s="17" t="inlineStr">
+      <c r="H110" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I110" s="20" t="n"/>
     </row>
     <row r="111">
       <c r="A111" s="4" t="inlineStr">
@@ -3425,8 +3664,10 @@
         </is>
       </c>
       <c r="E111" s="4" t="n"/>
-      <c r="F111" s="4" t="n"/>
-      <c r="G111" s="18" t="n"/>
+      <c r="F111" s="20" t="n"/>
+      <c r="G111" s="4" t="n"/>
+      <c r="H111" s="18" t="n"/>
+      <c r="I111" s="20" t="n"/>
     </row>
     <row r="112">
       <c r="A112" s="4" t="inlineStr">
@@ -3450,8 +3691,10 @@
         </is>
       </c>
       <c r="E112" s="4" t="n"/>
-      <c r="F112" s="4" t="n"/>
-      <c r="G112" s="18" t="n"/>
+      <c r="F112" s="20" t="n"/>
+      <c r="G112" s="4" t="n"/>
+      <c r="H112" s="18" t="n"/>
+      <c r="I112" s="20" t="n"/>
     </row>
     <row r="113">
       <c r="A113" s="4" t="inlineStr">
@@ -3475,8 +3718,10 @@
         </is>
       </c>
       <c r="E113" s="4" t="n"/>
-      <c r="F113" s="4" t="n"/>
-      <c r="G113" s="18" t="n"/>
+      <c r="F113" s="20" t="n"/>
+      <c r="G113" s="4" t="n"/>
+      <c r="H113" s="18" t="n"/>
+      <c r="I113" s="20" t="n"/>
     </row>
     <row r="114" ht="30" customHeight="1">
       <c r="A114" s="4" t="inlineStr">
@@ -3500,8 +3745,10 @@
         </is>
       </c>
       <c r="E114" s="4" t="n"/>
-      <c r="F114" s="4" t="n"/>
-      <c r="G114" s="18" t="n"/>
+      <c r="F114" s="20" t="n"/>
+      <c r="G114" s="4" t="n"/>
+      <c r="H114" s="18" t="n"/>
+      <c r="I114" s="20" t="n"/>
     </row>
     <row r="115">
       <c r="A115" s="4" t="inlineStr">
@@ -3525,8 +3772,10 @@
         </is>
       </c>
       <c r="E115" s="4" t="n"/>
-      <c r="F115" s="4" t="n"/>
-      <c r="G115" s="18" t="n"/>
+      <c r="F115" s="20" t="n"/>
+      <c r="G115" s="4" t="n"/>
+      <c r="H115" s="18" t="n"/>
+      <c r="I115" s="20" t="n"/>
     </row>
     <row r="116">
       <c r="A116" s="4" t="inlineStr">
@@ -3550,8 +3799,10 @@
         </is>
       </c>
       <c r="E116" s="4" t="n"/>
-      <c r="F116" s="4" t="n"/>
-      <c r="G116" s="18" t="n"/>
+      <c r="F116" s="20" t="n"/>
+      <c r="G116" s="4" t="n"/>
+      <c r="H116" s="18" t="n"/>
+      <c r="I116" s="20" t="n"/>
     </row>
     <row r="117" ht="30" customHeight="1">
       <c r="A117" s="4" t="inlineStr">
@@ -3575,8 +3826,10 @@
         </is>
       </c>
       <c r="E117" s="4" t="n"/>
-      <c r="F117" s="4" t="n"/>
-      <c r="G117" s="18" t="n"/>
+      <c r="F117" s="20" t="n"/>
+      <c r="G117" s="4" t="n"/>
+      <c r="H117" s="18" t="n"/>
+      <c r="I117" s="20" t="n"/>
     </row>
     <row r="118" ht="30" customHeight="1">
       <c r="A118" s="4" t="inlineStr">
@@ -3600,10 +3853,15 @@
         </is>
       </c>
       <c r="E118" s="4" t="n"/>
-      <c r="F118" s="4" t="n"/>
-      <c r="G118" s="18" t="n"/>
-    </row>
-    <row r="119"/>
+      <c r="F118" s="20" t="n"/>
+      <c r="G118" s="4" t="n"/>
+      <c r="H118" s="18" t="n"/>
+      <c r="I118" s="20" t="n"/>
+    </row>
+    <row r="119">
+      <c r="F119" s="20" t="n"/>
+      <c r="I119" s="20" t="n"/>
+    </row>
     <row r="120" ht="17" customHeight="1">
       <c r="A120" s="11" t="inlineStr">
         <is>
@@ -3614,7 +3872,9 @@
       <c r="C120" s="15" t="n"/>
       <c r="D120" s="15" t="n"/>
       <c r="E120" s="15" t="n"/>
-      <c r="F120" s="16" t="n"/>
+      <c r="F120" s="20" t="n"/>
+      <c r="G120" s="16" t="n"/>
+      <c r="I120" s="20" t="n"/>
     </row>
     <row r="121" ht="17" customHeight="1">
       <c r="A121" s="3" t="inlineStr">
@@ -3642,16 +3902,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F121" s="3" t="inlineStr">
+      <c r="F121" s="20" t="n"/>
+      <c r="G121" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G121" s="17" t="inlineStr">
+      <c r="H121" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I121" s="20" t="n"/>
     </row>
     <row r="122" ht="30" customHeight="1">
       <c r="A122" s="4" t="inlineStr">
@@ -3675,8 +3937,10 @@
         </is>
       </c>
       <c r="E122" s="4" t="n"/>
-      <c r="F122" s="4" t="n"/>
-      <c r="G122" s="18" t="n"/>
+      <c r="F122" s="20" t="n"/>
+      <c r="G122" s="4" t="n"/>
+      <c r="H122" s="18" t="n"/>
+      <c r="I122" s="20" t="n"/>
     </row>
     <row r="123">
       <c r="A123" s="4" t="inlineStr">
@@ -3700,8 +3964,10 @@
         </is>
       </c>
       <c r="E123" s="4" t="n"/>
-      <c r="F123" s="4" t="n"/>
-      <c r="G123" s="18" t="n"/>
+      <c r="F123" s="20" t="n"/>
+      <c r="G123" s="4" t="n"/>
+      <c r="H123" s="18" t="n"/>
+      <c r="I123" s="20" t="n"/>
     </row>
     <row r="124">
       <c r="A124" s="4" t="inlineStr">
@@ -3725,8 +3991,10 @@
         </is>
       </c>
       <c r="E124" s="4" t="n"/>
-      <c r="F124" s="4" t="n"/>
-      <c r="G124" s="18" t="n"/>
+      <c r="F124" s="20" t="n"/>
+      <c r="G124" s="4" t="n"/>
+      <c r="H124" s="18" t="n"/>
+      <c r="I124" s="20" t="n"/>
     </row>
     <row r="125">
       <c r="A125" s="4" t="inlineStr">
@@ -3750,8 +4018,10 @@
         </is>
       </c>
       <c r="E125" s="4" t="n"/>
-      <c r="F125" s="4" t="n"/>
-      <c r="G125" s="18" t="n"/>
+      <c r="F125" s="20" t="n"/>
+      <c r="G125" s="4" t="n"/>
+      <c r="H125" s="18" t="n"/>
+      <c r="I125" s="20" t="n"/>
     </row>
     <row r="126">
       <c r="A126" s="4" t="inlineStr">
@@ -3775,8 +4045,10 @@
         </is>
       </c>
       <c r="E126" s="4" t="n"/>
-      <c r="F126" s="4" t="n"/>
-      <c r="G126" s="18" t="n"/>
+      <c r="F126" s="20" t="n"/>
+      <c r="G126" s="4" t="n"/>
+      <c r="H126" s="18" t="n"/>
+      <c r="I126" s="20" t="n"/>
     </row>
     <row r="127">
       <c r="A127" s="4" t="inlineStr">
@@ -3800,8 +4072,10 @@
         </is>
       </c>
       <c r="E127" s="4" t="n"/>
-      <c r="F127" s="4" t="n"/>
-      <c r="G127" s="18" t="n"/>
+      <c r="F127" s="20" t="n"/>
+      <c r="G127" s="4" t="n"/>
+      <c r="H127" s="18" t="n"/>
+      <c r="I127" s="20" t="n"/>
     </row>
     <row r="128">
       <c r="A128" s="4" t="inlineStr">
@@ -3825,8 +4099,10 @@
         </is>
       </c>
       <c r="E128" s="4" t="n"/>
-      <c r="F128" s="4" t="n"/>
-      <c r="G128" s="18" t="n"/>
+      <c r="F128" s="20" t="n"/>
+      <c r="G128" s="4" t="n"/>
+      <c r="H128" s="18" t="n"/>
+      <c r="I128" s="20" t="n"/>
     </row>
     <row r="129">
       <c r="A129" s="4" t="inlineStr">
@@ -3850,8 +4126,10 @@
         </is>
       </c>
       <c r="E129" s="4" t="n"/>
-      <c r="F129" s="4" t="n"/>
-      <c r="G129" s="18" t="n"/>
+      <c r="F129" s="20" t="n"/>
+      <c r="G129" s="4" t="n"/>
+      <c r="H129" s="18" t="n"/>
+      <c r="I129" s="20" t="n"/>
     </row>
     <row r="130" ht="30" customHeight="1">
       <c r="A130" s="4" t="inlineStr">
@@ -3875,8 +4153,10 @@
         </is>
       </c>
       <c r="E130" s="4" t="n"/>
-      <c r="F130" s="4" t="n"/>
-      <c r="G130" s="18" t="n"/>
+      <c r="F130" s="20" t="n"/>
+      <c r="G130" s="4" t="n"/>
+      <c r="H130" s="18" t="n"/>
+      <c r="I130" s="20" t="n"/>
     </row>
     <row r="131" ht="30" customHeight="1">
       <c r="A131" s="4" t="inlineStr">
@@ -3900,8 +4180,10 @@
         </is>
       </c>
       <c r="E131" s="4" t="n"/>
-      <c r="F131" s="4" t="n"/>
-      <c r="G131" s="18" t="n"/>
+      <c r="F131" s="20" t="n"/>
+      <c r="G131" s="4" t="n"/>
+      <c r="H131" s="18" t="n"/>
+      <c r="I131" s="20" t="n"/>
     </row>
     <row r="132" ht="30" customHeight="1">
       <c r="A132" s="4" t="inlineStr">
@@ -3925,8 +4207,10 @@
         </is>
       </c>
       <c r="E132" s="4" t="n"/>
-      <c r="F132" s="4" t="n"/>
-      <c r="G132" s="18" t="n"/>
+      <c r="F132" s="20" t="n"/>
+      <c r="G132" s="4" t="n"/>
+      <c r="H132" s="18" t="n"/>
+      <c r="I132" s="20" t="n"/>
     </row>
     <row r="133" ht="30" customHeight="1">
       <c r="A133" s="4" t="inlineStr">
@@ -3950,8 +4234,10 @@
         </is>
       </c>
       <c r="E133" s="4" t="n"/>
-      <c r="F133" s="4" t="n"/>
-      <c r="G133" s="18" t="n"/>
+      <c r="F133" s="20" t="n"/>
+      <c r="G133" s="4" t="n"/>
+      <c r="H133" s="18" t="n"/>
+      <c r="I133" s="20" t="n"/>
     </row>
     <row r="134" ht="30" customHeight="1">
       <c r="A134" s="4" t="inlineStr">
@@ -3975,8 +4261,10 @@
         </is>
       </c>
       <c r="E134" s="4" t="n"/>
-      <c r="F134" s="4" t="n"/>
-      <c r="G134" s="18" t="n"/>
+      <c r="F134" s="20" t="n"/>
+      <c r="G134" s="4" t="n"/>
+      <c r="H134" s="18" t="n"/>
+      <c r="I134" s="20" t="n"/>
     </row>
     <row r="135" ht="45" customHeight="1">
       <c r="A135" s="4" t="inlineStr">
@@ -4000,10 +4288,15 @@
         </is>
       </c>
       <c r="E135" s="4" t="n"/>
-      <c r="F135" s="4" t="n"/>
-      <c r="G135" s="18" t="n"/>
-    </row>
-    <row r="136"/>
+      <c r="F135" s="20" t="n"/>
+      <c r="G135" s="4" t="n"/>
+      <c r="H135" s="18" t="n"/>
+      <c r="I135" s="20" t="n"/>
+    </row>
+    <row r="136">
+      <c r="F136" s="20" t="n"/>
+      <c r="I136" s="20" t="n"/>
+    </row>
     <row r="137" ht="17" customHeight="1">
       <c r="A137" s="11" t="inlineStr">
         <is>
@@ -4014,7 +4307,9 @@
       <c r="C137" s="15" t="n"/>
       <c r="D137" s="15" t="n"/>
       <c r="E137" s="15" t="n"/>
-      <c r="F137" s="16" t="n"/>
+      <c r="F137" s="20" t="n"/>
+      <c r="G137" s="16" t="n"/>
+      <c r="I137" s="20" t="n"/>
     </row>
     <row r="138" ht="17" customHeight="1">
       <c r="A138" s="3" t="inlineStr">
@@ -4042,16 +4337,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F138" s="3" t="inlineStr">
+      <c r="F138" s="20" t="n"/>
+      <c r="G138" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G138" s="17" t="inlineStr">
+      <c r="H138" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I138" s="20" t="n"/>
     </row>
     <row r="139">
       <c r="A139" s="4" t="inlineStr">
@@ -4075,8 +4372,10 @@
         </is>
       </c>
       <c r="E139" s="4" t="n"/>
-      <c r="F139" s="4" t="n"/>
-      <c r="G139" s="18" t="n"/>
+      <c r="F139" s="20" t="n"/>
+      <c r="G139" s="4" t="n"/>
+      <c r="H139" s="18" t="n"/>
+      <c r="I139" s="20" t="n"/>
     </row>
     <row r="140">
       <c r="A140" s="4" t="inlineStr">
@@ -4100,8 +4399,10 @@
         </is>
       </c>
       <c r="E140" s="4" t="n"/>
-      <c r="F140" s="4" t="n"/>
-      <c r="G140" s="18" t="n"/>
+      <c r="F140" s="20" t="n"/>
+      <c r="G140" s="4" t="n"/>
+      <c r="H140" s="18" t="n"/>
+      <c r="I140" s="20" t="n"/>
     </row>
     <row r="141">
       <c r="A141" s="4" t="inlineStr">
@@ -4125,8 +4426,10 @@
         </is>
       </c>
       <c r="E141" s="4" t="n"/>
-      <c r="F141" s="4" t="n"/>
-      <c r="G141" s="18" t="n"/>
+      <c r="F141" s="20" t="n"/>
+      <c r="G141" s="4" t="n"/>
+      <c r="H141" s="18" t="n"/>
+      <c r="I141" s="20" t="n"/>
     </row>
     <row r="142">
       <c r="A142" s="4" t="inlineStr">
@@ -4150,8 +4453,10 @@
         </is>
       </c>
       <c r="E142" s="4" t="n"/>
-      <c r="F142" s="4" t="n"/>
-      <c r="G142" s="18" t="n"/>
+      <c r="F142" s="20" t="n"/>
+      <c r="G142" s="4" t="n"/>
+      <c r="H142" s="18" t="n"/>
+      <c r="I142" s="20" t="n"/>
     </row>
     <row r="143">
       <c r="A143" s="4" t="inlineStr">
@@ -4175,8 +4480,10 @@
         </is>
       </c>
       <c r="E143" s="4" t="n"/>
-      <c r="F143" s="4" t="n"/>
-      <c r="G143" s="18" t="n"/>
+      <c r="F143" s="20" t="n"/>
+      <c r="G143" s="4" t="n"/>
+      <c r="H143" s="18" t="n"/>
+      <c r="I143" s="20" t="n"/>
     </row>
     <row r="144">
       <c r="A144" s="4" t="inlineStr">
@@ -4200,10 +4507,15 @@
         </is>
       </c>
       <c r="E144" s="4" t="n"/>
-      <c r="F144" s="4" t="n"/>
-      <c r="G144" s="18" t="n"/>
-    </row>
-    <row r="145"/>
+      <c r="F144" s="20" t="n"/>
+      <c r="G144" s="4" t="n"/>
+      <c r="H144" s="18" t="n"/>
+      <c r="I144" s="20" t="n"/>
+    </row>
+    <row r="145">
+      <c r="F145" s="20" t="n"/>
+      <c r="I145" s="20" t="n"/>
+    </row>
     <row r="146" ht="17" customHeight="1">
       <c r="A146" s="11" t="inlineStr">
         <is>
@@ -4214,7 +4526,9 @@
       <c r="C146" s="15" t="n"/>
       <c r="D146" s="15" t="n"/>
       <c r="E146" s="15" t="n"/>
-      <c r="F146" s="16" t="n"/>
+      <c r="F146" s="20" t="n"/>
+      <c r="G146" s="16" t="n"/>
+      <c r="I146" s="20" t="n"/>
     </row>
     <row r="147" ht="17" customHeight="1">
       <c r="A147" s="3" t="inlineStr">
@@ -4242,16 +4556,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F147" s="3" t="inlineStr">
+      <c r="F147" s="20" t="n"/>
+      <c r="G147" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G147" s="17" t="inlineStr">
+      <c r="H147" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I147" s="20" t="n"/>
     </row>
     <row r="148" ht="409.6" customHeight="1">
       <c r="A148" s="4" t="inlineStr">
@@ -4279,7 +4595,8 @@
           <t>FAIL</t>
         </is>
       </c>
-      <c r="F148" s="4" t="inlineStr">
+      <c r="F148" s="20" t="n"/>
+      <c r="G148" s="4" t="inlineStr">
         <is>
           <t>Test Case 12.1: Autosave Functionality
 After adding stakeholder information, polled the database. No entries found for the work completed.
@@ -4293,7 +4610,8 @@
 Fix the underlying sync issue — data must successfully save to the database.</t>
         </is>
       </c>
-      <c r="G148" s="18" t="n"/>
+      <c r="H148" s="18" t="n"/>
+      <c r="I148" s="20" t="n"/>
     </row>
     <row r="149">
       <c r="A149" s="4" t="inlineStr">
@@ -4317,8 +4635,10 @@
         </is>
       </c>
       <c r="E149" s="4" t="n"/>
-      <c r="F149" s="4" t="n"/>
-      <c r="G149" s="18" t="n"/>
+      <c r="F149" s="20" t="n"/>
+      <c r="G149" s="4" t="n"/>
+      <c r="H149" s="18" t="n"/>
+      <c r="I149" s="20" t="n"/>
     </row>
     <row r="150" ht="30" customHeight="1">
       <c r="A150" s="4" t="inlineStr">
@@ -4342,8 +4662,10 @@
         </is>
       </c>
       <c r="E150" s="4" t="n"/>
-      <c r="F150" s="4" t="n"/>
-      <c r="G150" s="18" t="n"/>
+      <c r="F150" s="20" t="n"/>
+      <c r="G150" s="4" t="n"/>
+      <c r="H150" s="18" t="n"/>
+      <c r="I150" s="20" t="n"/>
     </row>
     <row r="151">
       <c r="A151" s="4" t="inlineStr">
@@ -4367,8 +4689,10 @@
         </is>
       </c>
       <c r="E151" s="4" t="n"/>
-      <c r="F151" s="4" t="n"/>
-      <c r="G151" s="18" t="n"/>
+      <c r="F151" s="20" t="n"/>
+      <c r="G151" s="4" t="n"/>
+      <c r="H151" s="18" t="n"/>
+      <c r="I151" s="20" t="n"/>
     </row>
     <row r="152">
       <c r="A152" s="4" t="inlineStr">
@@ -4392,8 +4716,10 @@
         </is>
       </c>
       <c r="E152" s="4" t="n"/>
-      <c r="F152" s="4" t="n"/>
-      <c r="G152" s="18" t="n"/>
+      <c r="F152" s="20" t="n"/>
+      <c r="G152" s="4" t="n"/>
+      <c r="H152" s="18" t="n"/>
+      <c r="I152" s="20" t="n"/>
     </row>
     <row r="153" ht="30" customHeight="1">
       <c r="A153" s="4" t="inlineStr">
@@ -4417,8 +4743,10 @@
         </is>
       </c>
       <c r="E153" s="4" t="n"/>
-      <c r="F153" s="4" t="n"/>
-      <c r="G153" s="18" t="n"/>
+      <c r="F153" s="20" t="n"/>
+      <c r="G153" s="4" t="n"/>
+      <c r="H153" s="18" t="n"/>
+      <c r="I153" s="20" t="n"/>
     </row>
     <row r="154">
       <c r="A154" s="4" t="inlineStr">
@@ -4442,8 +4770,10 @@
         </is>
       </c>
       <c r="E154" s="4" t="n"/>
-      <c r="F154" s="4" t="n"/>
-      <c r="G154" s="18" t="n"/>
+      <c r="F154" s="20" t="n"/>
+      <c r="G154" s="4" t="n"/>
+      <c r="H154" s="18" t="n"/>
+      <c r="I154" s="20" t="n"/>
     </row>
     <row r="155" ht="30" customHeight="1">
       <c r="A155" s="4" t="inlineStr">
@@ -4467,8 +4797,10 @@
         </is>
       </c>
       <c r="E155" s="4" t="n"/>
-      <c r="F155" s="4" t="n"/>
-      <c r="G155" s="18" t="n"/>
+      <c r="F155" s="20" t="n"/>
+      <c r="G155" s="4" t="n"/>
+      <c r="H155" s="18" t="n"/>
+      <c r="I155" s="20" t="n"/>
     </row>
     <row r="156">
       <c r="A156" s="4" t="inlineStr">
@@ -4492,8 +4824,10 @@
         </is>
       </c>
       <c r="E156" s="4" t="n"/>
-      <c r="F156" s="4" t="n"/>
-      <c r="G156" s="18" t="n"/>
+      <c r="F156" s="20" t="n"/>
+      <c r="G156" s="4" t="n"/>
+      <c r="H156" s="18" t="n"/>
+      <c r="I156" s="20" t="n"/>
     </row>
     <row r="157">
       <c r="A157" s="4" t="inlineStr">
@@ -4517,8 +4851,10 @@
         </is>
       </c>
       <c r="E157" s="4" t="n"/>
-      <c r="F157" s="4" t="n"/>
-      <c r="G157" s="18" t="n"/>
+      <c r="F157" s="20" t="n"/>
+      <c r="G157" s="4" t="n"/>
+      <c r="H157" s="18" t="n"/>
+      <c r="I157" s="20" t="n"/>
     </row>
     <row r="158">
       <c r="A158" s="4" t="inlineStr">
@@ -4542,8 +4878,10 @@
         </is>
       </c>
       <c r="E158" s="4" t="n"/>
-      <c r="F158" s="4" t="n"/>
-      <c r="G158" s="18" t="n"/>
+      <c r="F158" s="20" t="n"/>
+      <c r="G158" s="4" t="n"/>
+      <c r="H158" s="18" t="n"/>
+      <c r="I158" s="20" t="n"/>
     </row>
     <row r="159">
       <c r="A159" s="4" t="inlineStr">
@@ -4567,10 +4905,15 @@
         </is>
       </c>
       <c r="E159" s="4" t="n"/>
-      <c r="F159" s="4" t="n"/>
-      <c r="G159" s="18" t="n"/>
-    </row>
-    <row r="160"/>
+      <c r="F159" s="20" t="n"/>
+      <c r="G159" s="4" t="n"/>
+      <c r="H159" s="18" t="n"/>
+      <c r="I159" s="20" t="n"/>
+    </row>
+    <row r="160">
+      <c r="F160" s="20" t="n"/>
+      <c r="I160" s="20" t="n"/>
+    </row>
     <row r="161" ht="17" customHeight="1">
       <c r="A161" s="11" t="inlineStr">
         <is>
@@ -4581,7 +4924,9 @@
       <c r="C161" s="15" t="n"/>
       <c r="D161" s="15" t="n"/>
       <c r="E161" s="15" t="n"/>
-      <c r="F161" s="16" t="n"/>
+      <c r="F161" s="20" t="n"/>
+      <c r="G161" s="16" t="n"/>
+      <c r="I161" s="20" t="n"/>
     </row>
     <row r="162" ht="17" customHeight="1">
       <c r="A162" s="3" t="inlineStr">
@@ -4609,16 +4954,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F162" s="3" t="inlineStr">
+      <c r="F162" s="20" t="n"/>
+      <c r="G162" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G162" s="17" t="inlineStr">
+      <c r="H162" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I162" s="20" t="n"/>
     </row>
     <row r="163">
       <c r="A163" s="4" t="inlineStr">
@@ -4642,8 +4989,10 @@
         </is>
       </c>
       <c r="E163" s="4" t="n"/>
-      <c r="F163" s="4" t="n"/>
-      <c r="G163" s="18" t="n"/>
+      <c r="F163" s="20" t="n"/>
+      <c r="G163" s="4" t="n"/>
+      <c r="H163" s="18" t="n"/>
+      <c r="I163" s="20" t="n"/>
     </row>
     <row r="164" ht="30" customHeight="1">
       <c r="A164" s="4" t="inlineStr">
@@ -4667,8 +5016,10 @@
         </is>
       </c>
       <c r="E164" s="4" t="n"/>
-      <c r="F164" s="4" t="n"/>
-      <c r="G164" s="18" t="n"/>
+      <c r="F164" s="20" t="n"/>
+      <c r="G164" s="4" t="n"/>
+      <c r="H164" s="18" t="n"/>
+      <c r="I164" s="20" t="n"/>
     </row>
     <row r="165" ht="30" customHeight="1">
       <c r="A165" s="4" t="inlineStr">
@@ -4692,8 +5043,10 @@
         </is>
       </c>
       <c r="E165" s="4" t="n"/>
-      <c r="F165" s="4" t="n"/>
-      <c r="G165" s="18" t="n"/>
+      <c r="F165" s="20" t="n"/>
+      <c r="G165" s="4" t="n"/>
+      <c r="H165" s="18" t="n"/>
+      <c r="I165" s="20" t="n"/>
     </row>
     <row r="166">
       <c r="A166" s="4" t="inlineStr">
@@ -4717,8 +5070,10 @@
         </is>
       </c>
       <c r="E166" s="4" t="n"/>
-      <c r="F166" s="4" t="n"/>
-      <c r="G166" s="18" t="n"/>
+      <c r="F166" s="20" t="n"/>
+      <c r="G166" s="4" t="n"/>
+      <c r="H166" s="18" t="n"/>
+      <c r="I166" s="20" t="n"/>
     </row>
     <row r="167" ht="30" customHeight="1">
       <c r="A167" s="4" t="inlineStr">
@@ -4742,8 +5097,10 @@
         </is>
       </c>
       <c r="E167" s="4" t="n"/>
-      <c r="F167" s="4" t="n"/>
-      <c r="G167" s="18" t="n"/>
+      <c r="F167" s="20" t="n"/>
+      <c r="G167" s="4" t="n"/>
+      <c r="H167" s="18" t="n"/>
+      <c r="I167" s="20" t="n"/>
     </row>
     <row r="168">
       <c r="A168" s="4" t="inlineStr">
@@ -4767,10 +5124,15 @@
         </is>
       </c>
       <c r="E168" s="4" t="n"/>
-      <c r="F168" s="4" t="n"/>
-      <c r="G168" s="18" t="n"/>
-    </row>
-    <row r="169"/>
+      <c r="F168" s="20" t="n"/>
+      <c r="G168" s="4" t="n"/>
+      <c r="H168" s="18" t="n"/>
+      <c r="I168" s="20" t="n"/>
+    </row>
+    <row r="169">
+      <c r="F169" s="20" t="n"/>
+      <c r="I169" s="20" t="n"/>
+    </row>
     <row r="170" ht="17" customHeight="1">
       <c r="A170" s="11" t="inlineStr">
         <is>
@@ -4781,7 +5143,9 @@
       <c r="C170" s="15" t="n"/>
       <c r="D170" s="15" t="n"/>
       <c r="E170" s="15" t="n"/>
-      <c r="F170" s="16" t="n"/>
+      <c r="F170" s="20" t="n"/>
+      <c r="G170" s="16" t="n"/>
+      <c r="I170" s="20" t="n"/>
     </row>
     <row r="171" ht="17" customHeight="1">
       <c r="A171" s="3" t="inlineStr">
@@ -4809,16 +5173,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F171" s="3" t="inlineStr">
+      <c r="F171" s="20" t="n"/>
+      <c r="G171" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G171" s="17" t="inlineStr">
+      <c r="H171" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I171" s="20" t="n"/>
     </row>
     <row r="172">
       <c r="A172" s="4" t="inlineStr">
@@ -4842,8 +5208,10 @@
         </is>
       </c>
       <c r="E172" s="4" t="n"/>
-      <c r="F172" s="4" t="n"/>
-      <c r="G172" s="18" t="n"/>
+      <c r="F172" s="20" t="n"/>
+      <c r="G172" s="4" t="n"/>
+      <c r="H172" s="18" t="n"/>
+      <c r="I172" s="20" t="n"/>
     </row>
     <row r="173">
       <c r="A173" s="4" t="inlineStr">
@@ -4867,8 +5235,10 @@
         </is>
       </c>
       <c r="E173" s="4" t="n"/>
-      <c r="F173" s="4" t="n"/>
-      <c r="G173" s="18" t="n"/>
+      <c r="F173" s="20" t="n"/>
+      <c r="G173" s="4" t="n"/>
+      <c r="H173" s="18" t="n"/>
+      <c r="I173" s="20" t="n"/>
     </row>
     <row r="174" ht="30" customHeight="1">
       <c r="A174" s="4" t="inlineStr">
@@ -4892,8 +5262,10 @@
         </is>
       </c>
       <c r="E174" s="4" t="n"/>
-      <c r="F174" s="4" t="n"/>
-      <c r="G174" s="18" t="n"/>
+      <c r="F174" s="20" t="n"/>
+      <c r="G174" s="4" t="n"/>
+      <c r="H174" s="18" t="n"/>
+      <c r="I174" s="20" t="n"/>
     </row>
     <row r="175">
       <c r="A175" s="4" t="inlineStr">
@@ -4917,8 +5289,10 @@
         </is>
       </c>
       <c r="E175" s="4" t="n"/>
-      <c r="F175" s="4" t="n"/>
-      <c r="G175" s="18" t="n"/>
+      <c r="F175" s="20" t="n"/>
+      <c r="G175" s="4" t="n"/>
+      <c r="H175" s="18" t="n"/>
+      <c r="I175" s="20" t="n"/>
     </row>
     <row r="176">
       <c r="A176" s="4" t="inlineStr">
@@ -4942,8 +5316,10 @@
         </is>
       </c>
       <c r="E176" s="4" t="n"/>
-      <c r="F176" s="4" t="n"/>
-      <c r="G176" s="18" t="n"/>
+      <c r="F176" s="20" t="n"/>
+      <c r="G176" s="4" t="n"/>
+      <c r="H176" s="18" t="n"/>
+      <c r="I176" s="20" t="n"/>
     </row>
     <row r="177" ht="30" customHeight="1">
       <c r="A177" s="4" t="inlineStr">
@@ -4967,8 +5343,10 @@
         </is>
       </c>
       <c r="E177" s="4" t="n"/>
-      <c r="F177" s="4" t="n"/>
-      <c r="G177" s="18" t="n"/>
+      <c r="F177" s="20" t="n"/>
+      <c r="G177" s="4" t="n"/>
+      <c r="H177" s="18" t="n"/>
+      <c r="I177" s="20" t="n"/>
     </row>
     <row r="178">
       <c r="A178" s="4" t="inlineStr">
@@ -4992,10 +5370,15 @@
         </is>
       </c>
       <c r="E178" s="4" t="n"/>
-      <c r="F178" s="4" t="n"/>
-      <c r="G178" s="18" t="n"/>
-    </row>
-    <row r="179"/>
+      <c r="F178" s="20" t="n"/>
+      <c r="G178" s="4" t="n"/>
+      <c r="H178" s="18" t="n"/>
+      <c r="I178" s="20" t="n"/>
+    </row>
+    <row r="179">
+      <c r="F179" s="20" t="n"/>
+      <c r="I179" s="20" t="n"/>
+    </row>
     <row r="180" ht="17" customHeight="1">
       <c r="A180" s="11" t="inlineStr">
         <is>
@@ -5006,7 +5389,9 @@
       <c r="C180" s="15" t="n"/>
       <c r="D180" s="15" t="n"/>
       <c r="E180" s="15" t="n"/>
-      <c r="F180" s="16" t="n"/>
+      <c r="F180" s="20" t="n"/>
+      <c r="G180" s="16" t="n"/>
+      <c r="I180" s="20" t="n"/>
     </row>
     <row r="181" ht="17" customHeight="1">
       <c r="A181" s="3" t="inlineStr">
@@ -5034,16 +5419,18 @@
           <t>Result</t>
         </is>
       </c>
-      <c r="F181" s="3" t="inlineStr">
+      <c r="F181" s="20" t="n"/>
+      <c r="G181" s="3" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G181" s="17" t="inlineStr">
+      <c r="H181" s="17" t="inlineStr">
         <is>
           <t>Retest</t>
         </is>
       </c>
+      <c r="I181" s="20" t="n"/>
     </row>
     <row r="182" ht="30" customHeight="1">
       <c r="A182" s="4" t="inlineStr">
@@ -5067,8 +5454,10 @@
         </is>
       </c>
       <c r="E182" s="4" t="n"/>
-      <c r="F182" s="4" t="n"/>
-      <c r="G182" s="18" t="n"/>
+      <c r="F182" s="20" t="n"/>
+      <c r="G182" s="4" t="n"/>
+      <c r="H182" s="18" t="n"/>
+      <c r="I182" s="20" t="n"/>
     </row>
     <row r="183" ht="30" customHeight="1">
       <c r="A183" s="4" t="inlineStr">
@@ -5092,8 +5481,10 @@
         </is>
       </c>
       <c r="E183" s="4" t="n"/>
-      <c r="F183" s="4" t="n"/>
-      <c r="G183" s="18" t="n"/>
+      <c r="F183" s="20" t="n"/>
+      <c r="G183" s="4" t="n"/>
+      <c r="H183" s="18" t="n"/>
+      <c r="I183" s="20" t="n"/>
     </row>
     <row r="184">
       <c r="A184" s="4" t="inlineStr">
@@ -5121,7 +5512,9 @@
           <t>Skip</t>
         </is>
       </c>
-      <c r="F184" s="5" t="n"/>
+      <c r="F184" s="20" t="n"/>
+      <c r="G184" s="5" t="n"/>
+      <c r="I184" s="20" t="n"/>
     </row>
     <row r="185" ht="45" customHeight="1">
       <c r="A185" s="4" t="inlineStr">
@@ -5137,7 +5530,9 @@
       <c r="C185" s="4" t="n"/>
       <c r="D185" s="4" t="n"/>
       <c r="E185" s="4" t="n"/>
-      <c r="F185" s="5" t="n"/>
+      <c r="F185" s="20" t="n"/>
+      <c r="G185" s="5" t="n"/>
+      <c r="I185" s="20" t="n"/>
     </row>
     <row r="186" ht="60" customHeight="1">
       <c r="A186" s="4" t="inlineStr">
@@ -5153,7 +5548,9 @@
       <c r="C186" s="4" t="n"/>
       <c r="D186" s="4" t="n"/>
       <c r="E186" s="4" t="n"/>
-      <c r="F186" s="5" t="n"/>
+      <c r="F186" s="20" t="n"/>
+      <c r="G186" s="5" t="n"/>
+      <c r="I186" s="20" t="n"/>
     </row>
     <row r="187" ht="45" customHeight="1">
       <c r="A187" s="4" t="inlineStr">
@@ -5169,7 +5566,9 @@
       <c r="C187" s="4" t="n"/>
       <c r="D187" s="4" t="n"/>
       <c r="E187" s="4" t="n"/>
-      <c r="F187" s="5" t="n"/>
+      <c r="F187" s="20" t="n"/>
+      <c r="G187" s="5" t="n"/>
+      <c r="I187" s="20" t="n"/>
     </row>
     <row r="188" ht="30" customHeight="1">
       <c r="A188" s="4" t="inlineStr">
@@ -5185,7 +5584,9 @@
       <c r="C188" s="4" t="n"/>
       <c r="D188" s="4" t="n"/>
       <c r="E188" s="4" t="n"/>
-      <c r="F188" s="5" t="n"/>
+      <c r="F188" s="20" t="n"/>
+      <c r="G188" s="5" t="n"/>
+      <c r="I188" s="20" t="n"/>
     </row>
     <row r="189" ht="45" customHeight="1">
       <c r="A189" s="4" t="inlineStr">
@@ -5201,7 +5602,9 @@
       <c r="C189" s="4" t="n"/>
       <c r="D189" s="4" t="n"/>
       <c r="E189" s="4" t="n"/>
-      <c r="F189" s="5" t="n"/>
+      <c r="F189" s="20" t="n"/>
+      <c r="G189" s="5" t="n"/>
+      <c r="I189" s="20" t="n"/>
     </row>
     <row r="190" ht="45" customHeight="1">
       <c r="A190" s="4" t="inlineStr">
@@ -5217,7 +5620,9 @@
       <c r="C190" s="4" t="n"/>
       <c r="D190" s="4" t="n"/>
       <c r="E190" s="4" t="n"/>
-      <c r="F190" s="5" t="n"/>
+      <c r="F190" s="20" t="n"/>
+      <c r="G190" s="5" t="n"/>
+      <c r="I190" s="20" t="n"/>
     </row>
     <row r="191" ht="60" customHeight="1">
       <c r="A191" s="4" t="inlineStr">
@@ -5233,7 +5638,9 @@
       <c r="C191" s="4" t="n"/>
       <c r="D191" s="4" t="n"/>
       <c r="E191" s="4" t="n"/>
-      <c r="F191" s="5" t="n"/>
+      <c r="F191" s="20" t="n"/>
+      <c r="G191" s="5" t="n"/>
+      <c r="I191" s="20" t="n"/>
     </row>
     <row r="192" ht="60" customHeight="1">
       <c r="A192" s="4" t="inlineStr">
@@ -5249,7 +5656,9 @@
       <c r="C192" s="4" t="n"/>
       <c r="D192" s="4" t="n"/>
       <c r="E192" s="4" t="n"/>
-      <c r="F192" s="5" t="n"/>
+      <c r="F192" s="20" t="n"/>
+      <c r="G192" s="5" t="n"/>
+      <c r="I192" s="20" t="n"/>
     </row>
     <row r="193" ht="45" customHeight="1">
       <c r="A193" s="4" t="inlineStr">
@@ -5265,7 +5674,9 @@
       <c r="C193" s="4" t="n"/>
       <c r="D193" s="4" t="n"/>
       <c r="E193" s="4" t="n"/>
-      <c r="F193" s="5" t="n"/>
+      <c r="F193" s="20" t="n"/>
+      <c r="G193" s="5" t="n"/>
+      <c r="I193" s="20" t="n"/>
     </row>
     <row r="194" ht="75" customHeight="1">
       <c r="A194" s="4" t="inlineStr">
@@ -5281,7 +5692,9 @@
       <c r="C194" s="4" t="n"/>
       <c r="D194" s="4" t="n"/>
       <c r="E194" s="4" t="n"/>
-      <c r="F194" s="5" t="n"/>
+      <c r="F194" s="20" t="n"/>
+      <c r="G194" s="5" t="n"/>
+      <c r="I194" s="20" t="n"/>
     </row>
     <row r="195" ht="60" customHeight="1">
       <c r="A195" s="4" t="inlineStr">
@@ -5297,7 +5710,9 @@
       <c r="C195" s="4" t="n"/>
       <c r="D195" s="4" t="n"/>
       <c r="E195" s="4" t="n"/>
-      <c r="F195" s="5" t="n"/>
+      <c r="F195" s="20" t="n"/>
+      <c r="G195" s="5" t="n"/>
+      <c r="I195" s="20" t="n"/>
     </row>
     <row r="196" ht="45" customHeight="1">
       <c r="A196" s="4" t="inlineStr">
@@ -5313,7 +5728,9 @@
       <c r="C196" s="4" t="n"/>
       <c r="D196" s="4" t="n"/>
       <c r="E196" s="4" t="n"/>
-      <c r="F196" s="5" t="n"/>
+      <c r="F196" s="20" t="n"/>
+      <c r="G196" s="5" t="n"/>
+      <c r="I196" s="20" t="n"/>
     </row>
     <row r="197" ht="60" customHeight="1">
       <c r="A197" s="4" t="inlineStr">
@@ -5329,7 +5746,9 @@
       <c r="C197" s="4" t="n"/>
       <c r="D197" s="4" t="n"/>
       <c r="E197" s="4" t="n"/>
-      <c r="F197" s="5" t="n"/>
+      <c r="F197" s="20" t="n"/>
+      <c r="G197" s="5" t="n"/>
+      <c r="I197" s="20" t="n"/>
     </row>
     <row r="198" ht="30" customHeight="1">
       <c r="A198" s="4" t="inlineStr">
@@ -5345,7 +5764,9 @@
       <c r="C198" s="4" t="n"/>
       <c r="D198" s="4" t="n"/>
       <c r="E198" s="4" t="n"/>
-      <c r="F198" s="5" t="n"/>
+      <c r="F198" s="20" t="n"/>
+      <c r="G198" s="5" t="n"/>
+      <c r="I198" s="20" t="n"/>
     </row>
     <row r="199" ht="60" customHeight="1">
       <c r="A199" s="4" t="inlineStr">
@@ -5361,7 +5782,9 @@
       <c r="C199" s="4" t="n"/>
       <c r="D199" s="4" t="n"/>
       <c r="E199" s="4" t="n"/>
-      <c r="F199" s="5" t="n"/>
+      <c r="F199" s="20" t="n"/>
+      <c r="G199" s="5" t="n"/>
+      <c r="I199" s="20" t="n"/>
     </row>
     <row r="200" ht="30" customHeight="1">
       <c r="A200" s="4" t="inlineStr">
@@ -5377,7 +5800,9 @@
       <c r="C200" s="4" t="n"/>
       <c r="D200" s="4" t="n"/>
       <c r="E200" s="4" t="n"/>
-      <c r="F200" s="5" t="n"/>
+      <c r="F200" s="20" t="n"/>
+      <c r="G200" s="5" t="n"/>
+      <c r="I200" s="20" t="n"/>
     </row>
     <row r="201">
       <c r="A201" s="4" t="inlineStr">
@@ -5389,7 +5814,9 @@
       <c r="C201" s="4" t="n"/>
       <c r="D201" s="4" t="n"/>
       <c r="E201" s="5" t="n"/>
-      <c r="F201" s="5" t="n"/>
+      <c r="F201" s="20" t="n"/>
+      <c r="G201" s="5" t="n"/>
+      <c r="I201" s="20" t="n"/>
     </row>
     <row r="202" ht="30" customHeight="1">
       <c r="A202" s="4" t="inlineStr">
@@ -5401,7 +5828,9 @@
       <c r="C202" s="4" t="n"/>
       <c r="D202" s="4" t="n"/>
       <c r="E202" s="5" t="n"/>
-      <c r="F202" s="5" t="n"/>
+      <c r="F202" s="20" t="n"/>
+      <c r="G202" s="5" t="n"/>
+      <c r="I202" s="20" t="n"/>
     </row>
     <row r="203" ht="30" customHeight="1">
       <c r="A203" s="4" t="inlineStr">
@@ -5413,15 +5842,17 @@
       <c r="C203" s="4" t="n"/>
       <c r="D203" s="4" t="n"/>
       <c r="E203" s="5" t="n"/>
-      <c r="F203" s="5" t="n"/>
+      <c r="F203" s="20" t="n"/>
+      <c r="G203" s="5" t="n"/>
+      <c r="I203" s="20" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="A170:F170"/>
     <mergeCell ref="A85:F85"/>
     <mergeCell ref="A161:F161"/>
+    <mergeCell ref="A137:F137"/>
     <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A137:F137"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="A146:F146"/>
     <mergeCell ref="A120:F120"/>

</xml_diff>